<commit_message>
Add MagIC export test
</commit_message>
<xml_diff>
--- a/client/modules/magic/actions/tests/output/test.xlsx
+++ b/client/modules/magic/actions/tests/output/test.xlsx
@@ -4,8 +4,14 @@
   <workbookPr date1904="false"/>
   <sheets>
     <sheet name="contribution" sheetId="1" r:id="rId1"/>
-    <sheet name="sites" sheetId="2" r:id="rId2"/>
-    <sheet name="specimens" sheetId="3" r:id="rId3"/>
+    <sheet name="locations" sheetId="2" r:id="rId2"/>
+    <sheet name="sites" sheetId="3" r:id="rId3"/>
+    <sheet name="samples" sheetId="4" r:id="rId4"/>
+    <sheet name="specimens" sheetId="5" r:id="rId5"/>
+    <sheet name="measurements" sheetId="6" r:id="rId6"/>
+    <sheet name="criteria" sheetId="7" r:id="rId7"/>
+    <sheet name="ages" sheetId="8" r:id="rId8"/>
+    <sheet name="images" sheetId="9" r:id="rId9"/>
   </sheets>
 </workbook>
 </file>
@@ -13,7 +19,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -35,25 +41,10 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
-      <color rgb="808080"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
       <b/>
     </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <b/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <color rgb="808080"/>
-    </font>
   </fonts>
-  <fills count="14">
+  <fills count="7">
     <fill>
       <patternFill patternType="none">
         <bgColor/>
@@ -67,36 +58,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFcccccc"/>
-        <bgColor/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFcccccc"/>
-        <bgColor/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFf2f2f2"/>
-        <bgColor/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFf2f2f2"/>
-        <bgColor/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFf2f2f2"/>
-        <bgColor/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFf2f2f2"/>
         <bgColor/>
       </patternFill>
     </fill>
@@ -124,20 +85,8 @@
         <bgColor/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFf2f2f2"/>
-        <bgColor/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFf2f2f2"/>
-        <bgColor/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="14">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -168,47 +117,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thick">
+      <left style="hair">
         <color auto="1"/>
       </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thick">
+      <right style="hair">
         <color auto="1"/>
       </right>
       <top style="hair">
         <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color rgb="FFf2f2f2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FFf2f2f2"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -216,29 +135,29 @@
       <left style="hair">
         <color auto="1"/>
       </left>
-      <right style="thick">
+      <right style="hair">
         <color auto="1"/>
       </right>
       <top style="hair">
         <color auto="1"/>
       </top>
-      <bottom style="hair">
+      <bottom style="thick">
         <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="thick">
         <color auto="1"/>
       </left>
-      <right style="thin">
+      <right style="hair">
         <color auto="1"/>
       </right>
-      <top style="hair">
-        <color rgb="FFf2f2f2"/>
+      <top style="thick">
+        <color auto="1"/>
       </top>
-      <bottom style="hair">
-        <color rgb="FFf2f2f2"/>
+      <bottom style="thick">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -249,86 +168,11 @@
       <right style="thick">
         <color auto="1"/>
       </right>
-      <top style="hair">
+      <top style="thick">
         <color auto="1"/>
       </top>
       <bottom style="thick">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color rgb="FFf2f2f2"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color rgb="FFcccccc"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color rgb="FFcccccc"/>
-      </left>
-      <right style="thick">
-        <color auto="1"/>
-      </right>
-      <top style="thick">
-        <color auto="1"/>
-      </top>
-      <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color auto="1"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FFf2f2f2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="hair">
-        <color rgb="FFf2f2f2"/>
-      </top>
-      <bottom style="hair">
-        <color rgb="FFf2f2f2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -336,45 +180,24 @@
   <cellStyleXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles>
@@ -711,40 +534,36 @@
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="sites" workbookViewId="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
         <v xml:space="preserve">Group:  </v>
       </c>
-      <c r="B1" s="4" t="str">
+      <c r="B1" s="3" t="str">
         <v>Contribution</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="str">
+      <c r="A2" s="4" t="str">
         <v xml:space="preserve">Name:  </v>
       </c>
-      <c r="B2" s="6" t="str">
+      <c r="B2" s="4" t="str">
         <v>MagIC Version</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="str">
+      <c r="A3" s="5" t="str">
         <v xml:space="preserve">Type:  </v>
       </c>
-      <c r="B3" s="8" t="str">
+      <c r="B3" s="4" t="str">
         <v>String</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="str">
+      <c r="A4" s="5" t="str">
         <v xml:space="preserve">Column:  </v>
       </c>
-      <c r="B4" s="10" t="str">
+      <c r="B4" s="5" t="str">
         <v>magic_version</v>
       </c>
     </row>
@@ -761,110 +580,132 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="sites" workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v xml:space="preserve">Group:  </v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v xml:space="preserve">Name:  </v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v xml:space="preserve">Type:  </v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="str">
+        <v xml:space="preserve">Column:  </v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="sites" workbookViewId="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="14.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
         <v xml:space="preserve">Group:  </v>
       </c>
-      <c r="B1" s="11" t="str">
+      <c r="B1" s="6" t="str">
         <v>Names</v>
       </c>
-      <c r="C1" s="12" t="str">
+      <c r="C1" s="7" t="str">
         <v/>
       </c>
-      <c r="D1" s="4" t="str">
+      <c r="D1" s="3" t="str">
         <v>Site</v>
       </c>
-      <c r="E1" s="11" t="str">
+      <c r="E1" s="6" t="str">
         <v>Result</v>
       </c>
-      <c r="F1" s="12" t="str">
+      <c r="F1" s="7" t="str">
         <v/>
       </c>
-      <c r="G1" s="4" t="str">
+      <c r="G1" s="3" t="str">
         <v>Metadata</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="str">
+      <c r="A2" s="4" t="str">
         <v xml:space="preserve">Name:  </v>
       </c>
-      <c r="B2" s="13" t="str">
+      <c r="B2" s="4" t="str">
         <v>Site Name</v>
       </c>
-      <c r="C2" s="6" t="str">
+      <c r="C2" s="4" t="str">
         <v>Location Name</v>
       </c>
-      <c r="D2" s="6" t="str">
+      <c r="D2" s="4" t="str">
         <v>Site Name Alternatives</v>
       </c>
-      <c r="E2" s="6" t="str">
+      <c r="E2" s="4" t="str">
         <v>Method Codes</v>
       </c>
-      <c r="F2" s="6" t="str">
+      <c r="F2" s="4" t="str">
         <v>Citation Names</v>
       </c>
-      <c r="G2" s="6" t="str">
+      <c r="G2" s="4" t="str">
         <v>Description</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="str">
+      <c r="A3" s="5" t="str">
         <v xml:space="preserve">Type:  </v>
       </c>
-      <c r="B3" s="8" t="str">
+      <c r="B3" s="4" t="str">
         <v>String</v>
       </c>
-      <c r="C3" s="8" t="str">
+      <c r="C3" s="4" t="str">
         <v>String</v>
       </c>
-      <c r="D3" s="8" t="str">
+      <c r="D3" s="4" t="str">
         <v>List</v>
       </c>
-      <c r="E3" s="8" t="str">
+      <c r="E3" s="4" t="str">
         <v>List</v>
       </c>
-      <c r="F3" s="8" t="str">
+      <c r="F3" s="4" t="str">
         <v>List</v>
       </c>
-      <c r="G3" s="8" t="str">
+      <c r="G3" s="4" t="str">
         <v>String</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="str">
+      <c r="A4" s="5" t="str">
         <v xml:space="preserve">Column:  </v>
       </c>
-      <c r="B4" s="10" t="str">
+      <c r="B4" s="5" t="str">
         <v>site</v>
       </c>
-      <c r="C4" s="10" t="str">
+      <c r="C4" s="5" t="str">
         <v>location</v>
       </c>
-      <c r="D4" s="10" t="str">
+      <c r="D4" s="5" t="str">
         <v>site_alternatives</v>
       </c>
-      <c r="E4" s="10" t="str">
+      <c r="E4" s="5" t="str">
         <v>method_codes</v>
       </c>
-      <c r="F4" s="10" t="str">
+      <c r="F4" s="5" t="str">
         <v>citations</v>
       </c>
-      <c r="G4" s="10" t="str">
+      <c r="G4" s="5" t="str">
         <v>description</v>
       </c>
     </row>
@@ -873,22 +714,16 @@
         <v/>
       </c>
       <c r="B5" s="2" t="str">
+        <v>lo1</v>
+      </c>
+      <c r="C5" s="2" t="str">
         <v>si2</v>
       </c>
-      <c r="C5" s="2" t="str">
-        <v>lo1</v>
-      </c>
       <c r="D5" s="2" t="str">
-        <v/>
+        <v>a</v>
       </c>
       <c r="E5" s="2" t="str">
         <v>code2,code1</v>
-      </c>
-      <c r="F5" s="2" t="str">
-        <v/>
-      </c>
-      <c r="G5" s="2" t="str">
-        <v>a</v>
       </c>
     </row>
     <row r="6">
@@ -902,114 +737,131 @@
         <v>lo1</v>
       </c>
       <c r="D6" s="2" t="str">
+        <v>10.1023/A1</v>
+      </c>
+      <c r="E6" s="2" t="str">
         <v>Kiln</v>
-      </c>
-      <c r="E6" s="2" t="str">
-        <v/>
-      </c>
-      <c r="F6" s="2" t="str">
-        <v>10.1023/A1</v>
-      </c>
-      <c r="G6" s="2" t="str">
-        <v/>
       </c>
     </row>
   </sheetData>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="sites" workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v xml:space="preserve">Group:  </v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v xml:space="preserve">Name:  </v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v xml:space="preserve">Type:  </v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="str">
+        <v xml:space="preserve">Column:  </v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="sites" workbookViewId="0"/>
   </sheetViews>
-  <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
         <v xml:space="preserve">Group:  </v>
       </c>
-      <c r="B1" s="11" t="str">
+      <c r="B1" s="6" t="str">
         <v>Names</v>
       </c>
-      <c r="C1" s="12" t="str">
+      <c r="C1" s="7" t="str">
         <v/>
       </c>
-      <c r="D1" s="4" t="str">
+      <c r="D1" s="3" t="str">
         <v>Specimen</v>
       </c>
-      <c r="E1" s="4" t="str">
+      <c r="E1" s="3" t="str">
         <v>Result</v>
       </c>
-      <c r="F1" s="4" t="str">
+      <c r="F1" s="3" t="str">
         <v>Geology</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="5" t="str">
+      <c r="A2" s="4" t="str">
         <v xml:space="preserve">Name:  </v>
       </c>
-      <c r="B2" s="13" t="str">
+      <c r="B2" s="4" t="str">
         <v>Specimen Name</v>
       </c>
-      <c r="C2" s="13" t="str">
+      <c r="C2" s="4" t="str">
         <v>Sample Name</v>
       </c>
-      <c r="D2" s="13" t="str">
+      <c r="D2" s="4" t="str">
         <v>Specimen IGSN</v>
       </c>
-      <c r="E2" s="13" t="str">
+      <c r="E2" s="4" t="str">
         <v>Citation Names</v>
       </c>
-      <c r="F2" s="13" t="str">
+      <c r="F2" s="4" t="str">
         <v>Dip</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="7" t="str">
+      <c r="A3" s="5" t="str">
         <v xml:space="preserve">Type:  </v>
       </c>
-      <c r="B3" s="14" t="str">
+      <c r="B3" s="4" t="str">
         <v>String</v>
       </c>
-      <c r="C3" s="8" t="str">
+      <c r="C3" s="4" t="str">
         <v>String</v>
       </c>
-      <c r="D3" s="8" t="str">
+      <c r="D3" s="4" t="str">
         <v>String</v>
       </c>
-      <c r="E3" s="8" t="str">
+      <c r="E3" s="4" t="str">
         <v>List</v>
       </c>
-      <c r="F3" s="8" t="str">
+      <c r="F3" s="4" t="str">
         <v>Number in Degrees</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="9" t="str">
+      <c r="A4" s="5" t="str">
         <v xml:space="preserve">Column:  </v>
       </c>
-      <c r="B4" s="10" t="str">
+      <c r="B4" s="5" t="str">
         <v>specimen</v>
       </c>
-      <c r="C4" s="10" t="str">
+      <c r="C4" s="5" t="str">
         <v>sample</v>
       </c>
-      <c r="D4" s="10" t="str">
+      <c r="D4" s="5" t="str">
         <v>igsn</v>
       </c>
-      <c r="E4" s="10" t="str">
+      <c r="E4" s="5" t="str">
         <v>citations</v>
       </c>
-      <c r="F4" s="10" t="str">
+      <c r="F4" s="5" t="str">
         <v>dip</v>
       </c>
     </row>
@@ -1017,40 +869,161 @@
       <c r="A5" s="2" t="str">
         <v/>
       </c>
-      <c r="B5" s="2" t="str">
+      <c r="B5" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="C5" s="2" t="str">
+        <v>igsn1</v>
+      </c>
+      <c r="D5" s="2" t="str">
         <v>sp1</v>
       </c>
-      <c r="C5" s="2" t="str">
+      <c r="E5" s="2" t="str">
         <v>sa1</v>
       </c>
-      <c r="D5" s="2" t="str">
-        <v>igsn1</v>
-      </c>
-      <c r="E5" s="2" t="str">
+      <c r="F5" s="2" t="str">
         <v>10.1023/A:1,This study</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1.2</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="str">
         <v/>
       </c>
-      <c r="B6" s="2" t="str">
+      <c r="B6" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="C6" s="2" t="str">
+        <v>igsn2</v>
+      </c>
+      <c r="D6" s="2" t="str">
         <v>sp2</v>
       </c>
-      <c r="C6" s="2" t="str">
+      <c r="E6" s="2" t="str">
         <v>sa1</v>
       </c>
-      <c r="D6" s="2" t="str">
-        <v>igsn2</v>
-      </c>
-      <c r="E6" s="2" t="str">
-        <v/>
-      </c>
-      <c r="F6" s="2">
-        <v>1.3</v>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="sites" workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v xml:space="preserve">Group:  </v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v xml:space="preserve">Name:  </v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v xml:space="preserve">Type:  </v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="str">
+        <v xml:space="preserve">Column:  </v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="sites" workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v xml:space="preserve">Group:  </v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v xml:space="preserve">Name:  </v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v xml:space="preserve">Type:  </v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="str">
+        <v xml:space="preserve">Column:  </v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="sites" workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v xml:space="preserve">Group:  </v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v xml:space="preserve">Name:  </v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v xml:space="preserve">Type:  </v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="str">
+        <v xml:space="preserve">Column:  </v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView showGridLines="1" tabSelected="sites" workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="str">
+        <v xml:space="preserve">Group:  </v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="str">
+        <v xml:space="preserve">Name:  </v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="str">
+        <v xml:space="preserve">Type:  </v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="str">
+        <v xml:space="preserve">Column:  </v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add upgrade next steps
</commit_message>
<xml_diff>
--- a/client/modules/magic/actions/tests/output/test.xlsx
+++ b/client/modules/magic/actions/tests/output/test.xlsx
@@ -1213,12 +1213,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A6"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="9.640625" customWidth="1"/>
+    <col min="2" max="2"/>
+    <col min="3" max="3"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1245,10 +1247,11 @@
       <c r="A5" s="11" t="str">
         <v/>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="11" t="str">
-        <v/>
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11" t="str">
+        <v>A</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use Data Importer for all MagIC Upload formats
</commit_message>
<xml_diff>
--- a/client/modules/magic/actions/tests/output/test.xlsx
+++ b/client/modules/magic/actions/tests/output/test.xlsx
@@ -1219,29 +1219,53 @@
   </sheetViews>
   <cols>
     <col min="1" max="1" width="9.640625" customWidth="1"/>
-    <col min="2" max="2"/>
-    <col min="3" max="3"/>
+    <col min="2" max="2" width="20.3515625" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="3" t="str">
         <v xml:space="preserve">Group: </v>
       </c>
+      <c r="B1" s="12" t="str">
+        <v>Names</v>
+      </c>
+      <c r="C1" s="4" t="str">
+        <v/>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="str">
         <v xml:space="preserve">Name: </v>
       </c>
+      <c r="B2" s="14" t="str">
+        <v>Measurement Number</v>
+      </c>
+      <c r="C2" s="6" t="str">
+        <v>Experiment Name</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="7" t="str">
         <v xml:space="preserve">Type: </v>
       </c>
+      <c r="B3" s="16" t="str">
+        <v>String</v>
+      </c>
+      <c r="C3" s="8" t="str">
+        <v>String</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="9" t="str">
         <v xml:space="preserve">Column: </v>
       </c>
+      <c r="B4" s="18" t="str">
+        <v>number</v>
+      </c>
+      <c r="C4" s="10" t="str">
+        <v>experiment</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="11" t="str">
@@ -1255,5 +1279,8 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
 </worksheet>
 </file>
</xml_diff>